<commit_message>
Added yahoo finance API and allowed for upload of excel data to add a stock
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>arnav@utexas.edu</t>
   </si>
   <si>
     <t>Short</t>
+  </si>
+  <si>
+    <t>dilan@utexas.edu</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -377,9 +380,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>